<commit_message>
adding 3D file list
</commit_message>
<xml_diff>
--- a/Automation/Toestellen_Lijst_DVDW.xlsx
+++ b/Automation/Toestellen_Lijst_DVDW.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/975cc8dd7505fcd1/Vives/Sem5/project_week/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EO-ICT\Projectweek\Iot-Lab\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{0027AE37-08D9-40F3-BCD0-71B0B591A552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{778EE77C-D701-4F21-BF9F-13C337D9C7A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F551BB80-C99F-4808-AA62-F2AD1B676332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCFC976D-2325-442E-A3EB-50C599BEF1DC}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20177" xr2:uid="{FCFC976D-2325-442E-A3EB-50C599BEF1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Elektrische boiler</t>
   </si>
@@ -146,6 +146,21 @@
   </si>
   <si>
     <t>Zigbee/zwave lights</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>DVDW plug</t>
+  </si>
+  <si>
+    <t>Bouw_lampen_plug_1</t>
+  </si>
+  <si>
+    <t>Bouw_lampen_plug_2</t>
   </si>
 </sst>
 </file>
@@ -195,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,26 +255,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -267,6 +282,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -581,424 +606,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DEF8FA-49BB-43E4-8A63-F8EE7FAA4710}">
-  <dimension ref="B1:S26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="167" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.69140625" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.3828125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="2"/>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="10" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="10" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="2"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="10" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="2"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="2"/>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="10" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="7" t="s">
         <v>23</v>
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="2"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="2"/>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="10" t="s">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="P14" s="1"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="2"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="2"/>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="10" t="s">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="2"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="2"/>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="10" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="2"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="10" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="2"/>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8" t="s">
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="10" t="s">
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="7" t="s">
         <v>19</v>
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="2"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="2"/>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="10" t="s">
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="2"/>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="10" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="2"/>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="10" t="s">
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N26" s="1"/>
@@ -1007,6 +1054,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="Q13:S17"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B8:C8"/>
@@ -1015,25 +1081,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="Q13:S17"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>